<commit_message>
Tạo mới file AnroidArchitecture
- Xử lý sheet [Overvew]
</commit_message>
<xml_diff>
--- a/00.Template/nn_ObjName_Overview_date.xlsx
+++ b/00.Template/nn_ObjName_Overview_date.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AndroidKnowledge\AndroidArchitecture\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AndroidKnowledge\00.Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07B47955-B237-4E3F-B628-8CE8EAF020E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D8826DE-007F-499B-81AB-B45CDAAC9D15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,9 +18,6 @@
     <sheet name="Details" sheetId="5" r:id="rId3"/>
     <sheet name="Ver.差分" sheetId="6" r:id="rId4"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId5"/>
-  </externalReferences>
   <definedNames>
     <definedName name="AAAA">#REF!</definedName>
     <definedName name="qqqq">#REF!</definedName>
@@ -126,10 +123,6 @@
     <phoneticPr fontId="5"/>
   </si>
   <si>
-    <t>Giới hạn ứng dụng</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
     <t>Item</t>
     <phoneticPr fontId="5"/>
   </si>
@@ -473,6 +466,29 @@
   <si>
     <t>Example</t>
     <phoneticPr fontId="29"/>
+  </si>
+  <si>
+    <r>
+      <t>Giới hạn ứng dụng của đối t</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>ư</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Meiryo UI"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>ợng</t>
+    </r>
+    <phoneticPr fontId="5"/>
   </si>
 </sst>
 </file>
@@ -1107,9 +1123,6 @@
     <xf numFmtId="0" fontId="19" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1120,200 +1133,203 @@
     <xf numFmtId="0" fontId="19" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="3" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="4" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="4" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="4" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="3" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="2" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="2" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="3" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="4" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="4" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="4" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="3" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1333,33 +1349,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="更新履歴"/>
-      <sheetName val="基本情報"/>
-      <sheetName val="Example"/>
-      <sheetName val="Example (XBE)"/>
-      <sheetName val="処理詳細"/>
-      <sheetName val="Ver.差分"/>
-      <sheetName val="比較表"/>
-      <sheetName val="運用方法"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1665,7 +1654,7 @@
         <v>5</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
@@ -1795,7 +1784,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" s="25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B1" s="26"/>
       <c r="C1" s="27"/>
@@ -1808,419 +1797,427 @@
         <v>11</v>
       </c>
       <c r="B2" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="105" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="36" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="36"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="38"/>
+      <c r="D2" s="105"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="37"/>
     </row>
     <row r="3" spans="1:6" s="30" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="39">
+      <c r="A3" s="38">
         <v>1</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="104"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="37"/>
+    </row>
+    <row r="4" spans="1:6" s="30" customFormat="1" ht="83.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="38">
+        <v>3</v>
+      </c>
+      <c r="B4" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="41"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="38"/>
-    </row>
-    <row r="4" spans="1:6" s="30" customFormat="1" ht="83.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="39">
-        <v>3</v>
-      </c>
-      <c r="B4" s="43" t="s">
+      <c r="C4" s="104" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="96"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="37"/>
+    </row>
+    <row r="5" spans="1:6" s="30" customFormat="1" ht="207.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="38">
+        <v>4</v>
+      </c>
+      <c r="B5" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="41" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="42"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="38"/>
-    </row>
-    <row r="5" spans="1:6" s="30" customFormat="1" ht="207.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="39">
-        <v>4</v>
-      </c>
-      <c r="B5" s="44" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="46"/>
+      <c r="C5" s="103"/>
+      <c r="D5" s="103"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="42"/>
     </row>
     <row r="6" spans="1:6" s="30" customFormat="1" ht="200.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="39">
+      <c r="A6" s="38">
         <v>5</v>
       </c>
-      <c r="B6" s="47" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="46"/>
+      <c r="B6" s="43" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="103"/>
+      <c r="D6" s="103"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="42"/>
     </row>
     <row r="7" spans="1:6" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="48">
+      <c r="A7" s="100">
         <v>6</v>
       </c>
-      <c r="B7" s="49" t="s">
+      <c r="B7" s="97" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="50" t="s">
+      <c r="C7" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="51" t="s">
+      <c r="D7" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="37"/>
-      <c r="F7" s="38"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="37"/>
     </row>
     <row r="8" spans="1:6" s="30" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="52"/>
-      <c r="B8" s="53"/>
-      <c r="C8" s="54"/>
-      <c r="D8" s="55"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="38"/>
+      <c r="A8" s="101"/>
+      <c r="B8" s="98"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="37"/>
     </row>
     <row r="9" spans="1:6" s="30" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A9" s="52"/>
-      <c r="B9" s="53"/>
-      <c r="C9" s="54"/>
-      <c r="D9" s="55"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="38"/>
+      <c r="A9" s="101"/>
+      <c r="B9" s="98"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="37"/>
     </row>
     <row r="10" spans="1:6" s="30" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A10" s="56"/>
-      <c r="B10" s="57"/>
-      <c r="C10" s="54"/>
-      <c r="D10" s="55"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="38"/>
+      <c r="A10" s="102"/>
+      <c r="B10" s="99"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="37"/>
     </row>
     <row r="11" spans="1:6" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="48">
+      <c r="A11" s="100">
         <v>7</v>
       </c>
-      <c r="B11" s="49" t="s">
+      <c r="B11" s="97" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="50" t="s">
+      <c r="C11" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="51" t="s">
+      <c r="D11" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="37"/>
-      <c r="F11" s="38"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="37"/>
     </row>
     <row r="12" spans="1:6" s="30" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="52"/>
-      <c r="B12" s="53"/>
-      <c r="C12" s="58"/>
-      <c r="D12" s="55"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="38"/>
+      <c r="A12" s="101"/>
+      <c r="B12" s="98"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="37"/>
     </row>
     <row r="13" spans="1:6" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="52"/>
-      <c r="B13" s="53"/>
-      <c r="C13" s="59"/>
-      <c r="D13" s="59"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="38"/>
+      <c r="A13" s="101"/>
+      <c r="B13" s="98"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="37"/>
     </row>
     <row r="14" spans="1:6" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="52"/>
-      <c r="B14" s="53"/>
-      <c r="C14" s="59"/>
-      <c r="D14" s="59"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="38"/>
+      <c r="A14" s="101"/>
+      <c r="B14" s="98"/>
+      <c r="C14" s="49"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="37"/>
     </row>
     <row r="15" spans="1:6" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="56"/>
-      <c r="B15" s="57"/>
-      <c r="C15" s="59"/>
-      <c r="D15" s="59"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="38"/>
+      <c r="A15" s="102"/>
+      <c r="B15" s="99"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="37"/>
     </row>
     <row r="16" spans="1:6" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="48">
+      <c r="A16" s="100">
         <v>8</v>
       </c>
-      <c r="B16" s="49" t="s">
+      <c r="B16" s="97" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="50" t="s">
+      <c r="C16" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="51" t="s">
+      <c r="D16" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="37"/>
-      <c r="F16" s="38"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="37"/>
     </row>
     <row r="17" spans="1:6" s="30" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A17" s="52"/>
-      <c r="B17" s="53"/>
-      <c r="C17" s="58"/>
-      <c r="D17" s="55"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="38"/>
+      <c r="A17" s="101"/>
+      <c r="B17" s="98"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="37"/>
     </row>
     <row r="18" spans="1:6" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="52"/>
-      <c r="B18" s="53"/>
-      <c r="C18" s="59"/>
-      <c r="D18" s="59"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="38"/>
+      <c r="A18" s="101"/>
+      <c r="B18" s="98"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="37"/>
     </row>
     <row r="19" spans="1:6" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="52"/>
-      <c r="B19" s="53"/>
-      <c r="C19" s="59"/>
-      <c r="D19" s="59"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="38"/>
+      <c r="A19" s="101"/>
+      <c r="B19" s="98"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="37"/>
     </row>
     <row r="20" spans="1:6" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="56"/>
-      <c r="B20" s="57"/>
-      <c r="C20" s="59"/>
-      <c r="D20" s="59"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="38"/>
+      <c r="A20" s="102"/>
+      <c r="B20" s="99"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="37"/>
     </row>
     <row r="21" spans="1:6" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="48">
+      <c r="A21" s="100">
         <v>8</v>
       </c>
-      <c r="B21" s="49" t="s">
+      <c r="B21" s="97" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="50" t="s">
+      <c r="C21" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="51" t="s">
+      <c r="D21" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="E21" s="37"/>
-      <c r="F21" s="38"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="37"/>
     </row>
     <row r="22" spans="1:6" s="30" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A22" s="52"/>
-      <c r="B22" s="53"/>
-      <c r="C22" s="58"/>
-      <c r="D22" s="55"/>
-      <c r="E22" s="37"/>
-      <c r="F22" s="38"/>
+      <c r="A22" s="101"/>
+      <c r="B22" s="98"/>
+      <c r="C22" s="48"/>
+      <c r="D22" s="47"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="37"/>
     </row>
     <row r="23" spans="1:6" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="52"/>
-      <c r="B23" s="53"/>
-      <c r="C23" s="59"/>
-      <c r="D23" s="59"/>
-      <c r="E23" s="37"/>
-      <c r="F23" s="38"/>
+      <c r="A23" s="101"/>
+      <c r="B23" s="98"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="37"/>
     </row>
     <row r="24" spans="1:6" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="52"/>
-      <c r="B24" s="53"/>
-      <c r="C24" s="59"/>
-      <c r="D24" s="59"/>
-      <c r="E24" s="37"/>
-      <c r="F24" s="38"/>
+      <c r="A24" s="101"/>
+      <c r="B24" s="98"/>
+      <c r="C24" s="49"/>
+      <c r="D24" s="49"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="37"/>
     </row>
     <row r="25" spans="1:6" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="56"/>
-      <c r="B25" s="57"/>
-      <c r="C25" s="59"/>
-      <c r="D25" s="59"/>
-      <c r="E25" s="37"/>
-      <c r="F25" s="38"/>
+      <c r="A25" s="102"/>
+      <c r="B25" s="99"/>
+      <c r="C25" s="49"/>
+      <c r="D25" s="49"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="37"/>
     </row>
     <row r="26" spans="1:6" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="48">
+      <c r="A26" s="100">
         <v>8</v>
       </c>
-      <c r="B26" s="49" t="s">
+      <c r="B26" s="97" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="50" t="s">
+      <c r="C26" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="D26" s="51" t="s">
+      <c r="D26" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="E26" s="37"/>
-      <c r="F26" s="38"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="37"/>
     </row>
     <row r="27" spans="1:6" s="30" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A27" s="52"/>
-      <c r="B27" s="53"/>
-      <c r="C27" s="58"/>
-      <c r="D27" s="55"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="38"/>
+      <c r="A27" s="101"/>
+      <c r="B27" s="98"/>
+      <c r="C27" s="48"/>
+      <c r="D27" s="47"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="37"/>
     </row>
     <row r="28" spans="1:6" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="52"/>
-      <c r="B28" s="53"/>
-      <c r="C28" s="59"/>
-      <c r="D28" s="59"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="38"/>
+      <c r="A28" s="101"/>
+      <c r="B28" s="98"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="49"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="37"/>
     </row>
     <row r="29" spans="1:6" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="52"/>
-      <c r="B29" s="53"/>
-      <c r="C29" s="59"/>
-      <c r="D29" s="59"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="38"/>
+      <c r="A29" s="101"/>
+      <c r="B29" s="98"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="49"/>
+      <c r="E29" s="36"/>
+      <c r="F29" s="37"/>
     </row>
     <row r="30" spans="1:6" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="56"/>
-      <c r="B30" s="57"/>
-      <c r="C30" s="59"/>
-      <c r="D30" s="59"/>
-      <c r="E30" s="37"/>
-      <c r="F30" s="38"/>
+      <c r="A30" s="102"/>
+      <c r="B30" s="99"/>
+      <c r="C30" s="49"/>
+      <c r="D30" s="49"/>
+      <c r="E30" s="36"/>
+      <c r="F30" s="37"/>
     </row>
     <row r="31" spans="1:6" s="30" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A31" s="39">
+      <c r="A31" s="38">
         <v>9</v>
       </c>
-      <c r="B31" s="44" t="s">
+      <c r="B31" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="C31" s="41"/>
-      <c r="D31" s="42"/>
-      <c r="E31" s="37"/>
-      <c r="F31" s="38"/>
+      <c r="C31" s="104"/>
+      <c r="D31" s="96"/>
+      <c r="E31" s="36"/>
+      <c r="F31" s="37"/>
     </row>
     <row r="32" spans="1:6" s="30" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A32" s="39">
+      <c r="A32" s="38">
         <v>10</v>
       </c>
       <c r="B32" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="C32" s="60"/>
-      <c r="D32" s="42"/>
-      <c r="E32" s="37"/>
-      <c r="F32" s="38"/>
+      <c r="C32" s="95"/>
+      <c r="D32" s="96"/>
+      <c r="E32" s="36"/>
+      <c r="F32" s="37"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="61"/>
-      <c r="B33" s="62"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="37"/>
-      <c r="F33" s="38"/>
+      <c r="A33" s="50"/>
+      <c r="B33" s="51"/>
+      <c r="C33" s="37"/>
+      <c r="D33" s="37"/>
+      <c r="E33" s="36"/>
+      <c r="F33" s="37"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="61"/>
-      <c r="B34" s="62"/>
-      <c r="C34" s="38"/>
-      <c r="D34" s="38"/>
-      <c r="E34" s="37"/>
-      <c r="F34" s="38"/>
+      <c r="A34" s="50"/>
+      <c r="B34" s="51"/>
+      <c r="C34" s="37"/>
+      <c r="D34" s="37"/>
+      <c r="E34" s="36"/>
+      <c r="F34" s="37"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="61"/>
-      <c r="B35" s="62"/>
-      <c r="C35" s="38"/>
-      <c r="D35" s="38"/>
-      <c r="E35" s="37"/>
-      <c r="F35" s="38"/>
+      <c r="A35" s="50"/>
+      <c r="B35" s="51"/>
+      <c r="C35" s="37"/>
+      <c r="D35" s="37"/>
+      <c r="E35" s="36"/>
+      <c r="F35" s="37"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="61"/>
-      <c r="B36" s="62"/>
-      <c r="C36" s="38"/>
-      <c r="D36" s="38"/>
-      <c r="E36" s="37"/>
-      <c r="F36" s="38"/>
+      <c r="A36" s="50"/>
+      <c r="B36" s="51"/>
+      <c r="C36" s="37"/>
+      <c r="D36" s="37"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="37"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="61"/>
-      <c r="B37" s="62"/>
-      <c r="C37" s="38"/>
-      <c r="D37" s="38"/>
-      <c r="E37" s="37"/>
-      <c r="F37" s="38"/>
+      <c r="A37" s="50"/>
+      <c r="B37" s="51"/>
+      <c r="C37" s="37"/>
+      <c r="D37" s="37"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="37"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="61"/>
-      <c r="B38" s="62"/>
-      <c r="C38" s="38"/>
-      <c r="D38" s="38"/>
-      <c r="E38" s="37"/>
-      <c r="F38" s="38"/>
+      <c r="A38" s="50"/>
+      <c r="B38" s="51"/>
+      <c r="C38" s="37"/>
+      <c r="D38" s="37"/>
+      <c r="E38" s="36"/>
+      <c r="F38" s="37"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="61"/>
-      <c r="B39" s="62"/>
-      <c r="C39" s="38"/>
-      <c r="D39" s="38"/>
-      <c r="E39" s="37"/>
-      <c r="F39" s="38"/>
+      <c r="A39" s="50"/>
+      <c r="B39" s="51"/>
+      <c r="C39" s="37"/>
+      <c r="D39" s="37"/>
+      <c r="E39" s="36"/>
+      <c r="F39" s="37"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="61"/>
-      <c r="B40" s="62"/>
-      <c r="C40" s="38"/>
-      <c r="D40" s="38"/>
-      <c r="E40" s="37"/>
-      <c r="F40" s="38"/>
+      <c r="A40" s="50"/>
+      <c r="B40" s="51"/>
+      <c r="C40" s="37"/>
+      <c r="D40" s="37"/>
+      <c r="E40" s="36"/>
+      <c r="F40" s="37"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="61"/>
-      <c r="B41" s="62"/>
-      <c r="C41" s="38"/>
-      <c r="D41" s="38"/>
-      <c r="E41" s="37"/>
-      <c r="F41" s="38"/>
+      <c r="A41" s="50"/>
+      <c r="B41" s="51"/>
+      <c r="C41" s="37"/>
+      <c r="D41" s="37"/>
+      <c r="E41" s="36"/>
+      <c r="F41" s="37"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="61"/>
-      <c r="B42" s="62"/>
-      <c r="C42" s="38"/>
-      <c r="D42" s="38"/>
-      <c r="E42" s="37"/>
-      <c r="F42" s="38"/>
+      <c r="A42" s="50"/>
+      <c r="B42" s="51"/>
+      <c r="C42" s="37"/>
+      <c r="D42" s="37"/>
+      <c r="E42" s="36"/>
+      <c r="F42" s="37"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="61"/>
-      <c r="B43" s="62"/>
-      <c r="C43" s="38"/>
-      <c r="D43" s="38"/>
-      <c r="E43" s="37"/>
-      <c r="F43" s="38"/>
+      <c r="A43" s="50"/>
+      <c r="B43" s="51"/>
+      <c r="C43" s="37"/>
+      <c r="D43" s="37"/>
+      <c r="E43" s="36"/>
+      <c r="F43" s="37"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A44" s="63"/>
-      <c r="B44" s="64"/>
-      <c r="C44" s="65"/>
-      <c r="D44" s="65"/>
-      <c r="E44" s="66"/>
-      <c r="F44" s="65"/>
+      <c r="A44" s="52"/>
+      <c r="B44" s="53"/>
+      <c r="C44" s="54"/>
+      <c r="D44" s="54"/>
+      <c r="E44" s="55"/>
+      <c r="F44" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A11:A15"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="B11:B15"/>
     <mergeCell ref="B7:B10"/>
@@ -2230,14 +2227,6 @@
     <mergeCell ref="B21:B25"/>
     <mergeCell ref="A26:A30"/>
     <mergeCell ref="B26:B30"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="A11:A15"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2257,145 +2246,145 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="2.25" style="71" customWidth="1"/>
-    <col min="2" max="2" width="4.25" style="72" customWidth="1"/>
-    <col min="3" max="3" width="18.125" style="72" customWidth="1"/>
-    <col min="4" max="4" width="17.25" style="71" customWidth="1"/>
-    <col min="5" max="5" width="13.625" style="72" customWidth="1"/>
-    <col min="6" max="6" width="31" style="72" customWidth="1"/>
-    <col min="7" max="7" width="73.125" style="71" customWidth="1"/>
-    <col min="8" max="8" width="42.625" style="71" customWidth="1"/>
-    <col min="9" max="16384" width="9.125" style="71"/>
+    <col min="1" max="1" width="2.25" style="60" customWidth="1"/>
+    <col min="2" max="2" width="4.25" style="61" customWidth="1"/>
+    <col min="3" max="3" width="18.125" style="61" customWidth="1"/>
+    <col min="4" max="4" width="17.25" style="60" customWidth="1"/>
+    <col min="5" max="5" width="13.625" style="61" customWidth="1"/>
+    <col min="6" max="6" width="31" style="61" customWidth="1"/>
+    <col min="7" max="7" width="73.125" style="60" customWidth="1"/>
+    <col min="8" max="8" width="42.625" style="60" customWidth="1"/>
+    <col min="9" max="16384" width="9.125" style="60"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="B1" s="69" t="s">
-        <v>38</v>
-      </c>
-      <c r="C1" s="70"/>
+      <c r="B1" s="58" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="59"/>
     </row>
     <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="3" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="73" t="s">
+      <c r="B3" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="74" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" s="74" t="s">
-        <v>39</v>
-      </c>
-      <c r="E3" s="74" t="s">
+      <c r="C3" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="74" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" s="74" t="s">
+      <c r="D3" s="63" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="63" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="63" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="63" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3" s="64" t="s">
         <v>43</v>
       </c>
-      <c r="H3" s="75" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="4" spans="2:8" ht="57" x14ac:dyDescent="0.4">
-      <c r="B4" s="76">
+      <c r="B4" s="65">
         <f>ROW()-3</f>
         <v>1</v>
       </c>
-      <c r="C4" s="68" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4" s="68" t="s">
+      <c r="C4" s="57" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="57" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="66" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="67"/>
+      <c r="G4" s="70" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="77" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" s="78"/>
-      <c r="G4" s="81" t="s">
-        <v>41</v>
-      </c>
-      <c r="H4" s="79"/>
+      <c r="H4" s="68"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B5" s="76">
+      <c r="B5" s="65">
         <f t="shared" ref="B5:B9" si="0">ROW()-3</f>
         <v>2</v>
       </c>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" s="77" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" s="78"/>
-      <c r="G5" s="68" t="s">
-        <v>42</v>
-      </c>
-      <c r="H5" s="79"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="66" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="67"/>
+      <c r="G5" s="57" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" s="68"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B6" s="76">
+      <c r="B6" s="65">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="C6" s="80"/>
-      <c r="D6" s="68"/>
-      <c r="E6" s="77"/>
-      <c r="F6" s="78"/>
-      <c r="G6" s="68"/>
-      <c r="H6" s="79"/>
+      <c r="C6" s="69"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="57"/>
+      <c r="H6" s="68"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B7" s="76">
+      <c r="B7" s="65">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C7" s="80"/>
-      <c r="D7" s="68"/>
-      <c r="E7" s="77"/>
-      <c r="F7" s="78"/>
-      <c r="G7" s="68"/>
-      <c r="H7" s="79"/>
+      <c r="C7" s="69"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="57"/>
+      <c r="H7" s="68"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B8" s="76">
+      <c r="B8" s="65">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C8" s="80"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="77"/>
-      <c r="F8" s="78"/>
-      <c r="G8" s="68"/>
-      <c r="H8" s="79"/>
+      <c r="C8" s="69"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="66"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="57"/>
+      <c r="H8" s="68"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B9" s="76">
+      <c r="B9" s="65">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C9" s="80"/>
-      <c r="D9" s="68"/>
-      <c r="E9" s="77"/>
-      <c r="F9" s="78"/>
-      <c r="G9" s="68"/>
-      <c r="H9" s="79"/>
+      <c r="C9" s="69"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="66"/>
+      <c r="F9" s="67"/>
+      <c r="G9" s="57"/>
+      <c r="H9" s="68"/>
     </row>
     <row r="10" spans="2:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B10" s="82" t="s">
+      <c r="B10" s="71" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="72" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="83" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="84"/>
-      <c r="E10" s="84"/>
-      <c r="F10" s="84"/>
-      <c r="G10" s="84"/>
-      <c r="H10" s="85"/>
+      <c r="D10" s="73"/>
+      <c r="E10" s="73"/>
+      <c r="F10" s="73"/>
+      <c r="G10" s="73"/>
+      <c r="H10" s="74"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3"/>
@@ -2426,88 +2415,88 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="2.25" style="67" customWidth="1"/>
-    <col min="2" max="2" width="3.75" style="90" customWidth="1"/>
-    <col min="3" max="3" width="8.375" style="90" customWidth="1"/>
-    <col min="4" max="4" width="32.25" style="91" customWidth="1"/>
-    <col min="5" max="5" width="7.125" style="88" customWidth="1"/>
-    <col min="6" max="6" width="55.375" style="92" customWidth="1"/>
-    <col min="7" max="7" width="38.875" style="67" customWidth="1"/>
-    <col min="8" max="8" width="49" style="67" customWidth="1"/>
-    <col min="9" max="9" width="8.5" style="90" customWidth="1"/>
-    <col min="10" max="10" width="17.375" style="90" customWidth="1"/>
-    <col min="11" max="16384" width="9" style="67"/>
+    <col min="1" max="1" width="2.25" style="56" customWidth="1"/>
+    <col min="2" max="2" width="3.75" style="79" customWidth="1"/>
+    <col min="3" max="3" width="8.375" style="79" customWidth="1"/>
+    <col min="4" max="4" width="32.25" style="80" customWidth="1"/>
+    <col min="5" max="5" width="7.125" style="77" customWidth="1"/>
+    <col min="6" max="6" width="55.375" style="81" customWidth="1"/>
+    <col min="7" max="7" width="38.875" style="56" customWidth="1"/>
+    <col min="8" max="8" width="49" style="56" customWidth="1"/>
+    <col min="9" max="9" width="8.5" style="79" customWidth="1"/>
+    <col min="10" max="10" width="17.375" style="79" customWidth="1"/>
+    <col min="11" max="16384" width="9" style="56"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="71"/>
-      <c r="B1" s="93" t="s">
+      <c r="A1" s="60"/>
+      <c r="B1" s="82" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A2" s="60"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="87"/>
+      <c r="G2" s="87"/>
+      <c r="H2" s="87"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="56"/>
+    </row>
+    <row r="3" spans="1:10" ht="28.5" x14ac:dyDescent="0.4">
+      <c r="A3" s="60"/>
+      <c r="B3" s="88" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="95"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="67"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A2" s="71"/>
-      <c r="B2" s="96"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="67"/>
-    </row>
-    <row r="3" spans="1:10" ht="28.5" x14ac:dyDescent="0.4">
-      <c r="A3" s="71"/>
-      <c r="B3" s="99" t="s">
+      <c r="C3" s="89" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="89" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="89" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="100" t="s">
-        <v>48</v>
-      </c>
-      <c r="D3" s="100" t="s">
+      <c r="F3" s="89" t="s">
         <v>49</v>
       </c>
-      <c r="E3" s="100" t="s">
-        <v>47</v>
-      </c>
-      <c r="F3" s="100" t="s">
+      <c r="G3" s="88" t="s">
         <v>50</v>
       </c>
-      <c r="G3" s="99" t="s">
+      <c r="H3" s="88" t="s">
         <v>51</v>
       </c>
-      <c r="H3" s="99" t="s">
+      <c r="I3" s="76" t="s">
         <v>52</v>
       </c>
-      <c r="I3" s="87" t="s">
-        <v>53</v>
-      </c>
-      <c r="J3" s="88"/>
+      <c r="J3" s="77"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A4" s="71"/>
-      <c r="B4" s="101">
+      <c r="A4" s="60"/>
+      <c r="B4" s="90">
         <f>ROW()-3</f>
         <v>1</v>
       </c>
-      <c r="C4" s="77" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="102"/>
-      <c r="E4" s="103"/>
-      <c r="F4" s="104"/>
-      <c r="G4" s="68"/>
-      <c r="H4" s="105"/>
-      <c r="I4" s="89" t="str">
+      <c r="C4" s="66" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="91"/>
+      <c r="E4" s="92"/>
+      <c r="F4" s="93"/>
+      <c r="G4" s="57"/>
+      <c r="H4" s="94"/>
+      <c r="I4" s="78" t="str">
         <f ca="1">HYPERLINK("["&amp;SUBSTITUTE(CELL("filename"),TRIM(RIGHT(SUBSTITUTE(CELL("filename"),"\",REPT(" ",255)),255)),"")&amp;"Samples\No"&amp;B4&amp;".xlsx]","click")</f>
         <v>click</v>
       </c>

</xml_diff>

<commit_message>
Thêm Overview Android Component
Xử lý được 1/2 nội dung cần làm ở sheet [Overview]
</commit_message>
<xml_diff>
--- a/00.Template/nn_ObjName_Overview_date.xlsx
+++ b/00.Template/nn_ObjName_Overview_date.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AndroidKnowledge\00.Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D8826DE-007F-499B-81AB-B45CDAAC9D15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4BE95FE-E851-4E68-8B2B-329DF1B61464}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -283,148 +283,6 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <r>
-      <t>Tên đối t</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>ư</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Meiryo UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>ợng</t>
-    </r>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <r>
-      <t>đối t</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>ư</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Meiryo UI"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>ợng tham gia</t>
-    </r>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Meiryo UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>Tên flow đối t</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>ư</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Meiryo UI"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">ợng tham gia là gì?
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Meiryo UI"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Meiryo UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>&lt;Mô tả flow mà đối t</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>ư</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Meiryo UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>ợng tham gia&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Meiryo UI"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <r>
-      <t>&lt;Mô tả flow xử lý nội bộ của đối t</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>ư</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Meiryo UI"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>ợng&gt;</t>
-    </r>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>Thông tin chi tiết</t>
     <phoneticPr fontId="5"/>
   </si>
@@ -441,7 +299,7 @@
   </si>
   <si>
     <t>Ver.</t>
-    <phoneticPr fontId="29"/>
+    <phoneticPr fontId="21"/>
   </si>
   <si>
     <t>Phân loại</t>
@@ -453,19 +311,19 @@
   </si>
   <si>
     <t>Path</t>
-    <phoneticPr fontId="29"/>
+    <phoneticPr fontId="21"/>
   </si>
   <si>
     <t>Thông tin chi tiết</t>
-    <phoneticPr fontId="29"/>
+    <phoneticPr fontId="21"/>
   </si>
   <si>
     <t>Ghi chú</t>
-    <phoneticPr fontId="29"/>
+    <phoneticPr fontId="21"/>
   </si>
   <si>
     <t>Example</t>
-    <phoneticPr fontId="29"/>
+    <phoneticPr fontId="21"/>
   </si>
   <si>
     <r>
@@ -490,12 +348,134 @@
     </r>
     <phoneticPr fontId="5"/>
   </si>
+  <si>
+    <t>Thành phần cụ thể</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <r>
+      <t>đối t</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>ư</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Meiryo UI"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>ợng tham gia</t>
+    </r>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Meiryo UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tên flow đối t</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>ư</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Meiryo UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ợng tham gia là gì?
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Meiryo UI"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Meiryo UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>&lt;Mô tả flow mà đối t</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>ư</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Meiryo UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>ợng tham gia&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Meiryo UI"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <r>
+      <t>&lt;Mô tả flow xử lý nội bộ của đối t</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>ư</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Meiryo UI"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>ợng&gt;</t>
+    </r>
+    <phoneticPr fontId="3"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="32" x14ac:knownFonts="1">
+  <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -583,12 +563,6 @@
       <charset val="128"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Meiryo UI"/>
-      <family val="2"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
@@ -597,11 +571,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="16"/>
       <name val="Meiryo UI"/>
@@ -645,46 +614,11 @@
       <charset val="128"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="0" tint="-0.499984740745262"/>
-      <name val="Meiryo UI"/>
-      <family val="3"/>
-      <charset val="128"/>
-    </font>
-    <font>
       <b/>
       <sz val="10"/>
       <name val="Meiryo UI"/>
       <family val="3"/>
       <charset val="128"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="Courier New"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Meiryo UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Meiryo UI"/>
-      <family val="2"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color theme="0" tint="-0.499984740745262"/>
-      <name val="Courier New"/>
-      <family val="3"/>
     </font>
     <font>
       <b/>
@@ -695,17 +629,59 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <u/>
       <sz val="10"/>
-      <color rgb="FF0000FF"/>
       <name val="Meiryo UI"/>
       <family val="3"/>
       <charset val="128"/>
     </font>
     <font>
       <b/>
+      <sz val="8"/>
+      <name val="Meiryo UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Meiryo UI"/>
+      <family val="2"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Meiryo UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Meiryo UI"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <name val="Meiryo UI"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
       <u/>
-      <sz val="10"/>
+      <sz val="8"/>
+      <color rgb="FF0000FF"/>
       <name val="Meiryo UI"/>
       <family val="3"/>
       <charset val="128"/>
@@ -1015,7 +991,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1092,105 +1068,102 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="3" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="3" applyFont="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="3" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="3" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1">
@@ -1199,137 +1172,140 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="2" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="4" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="3" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="4" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="4" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="4" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="3" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="2" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1799,10 +1775,10 @@
       <c r="B2" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="105" t="s">
+      <c r="C2" s="78" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="105"/>
+      <c r="D2" s="78"/>
       <c r="E2" s="36"/>
       <c r="F2" s="37"/>
     </row>
@@ -1813,8 +1789,8 @@
       <c r="B3" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="104"/>
-      <c r="D3" s="96"/>
+      <c r="C3" s="76"/>
+      <c r="D3" s="77"/>
       <c r="E3" s="36"/>
       <c r="F3" s="37"/>
     </row>
@@ -1825,10 +1801,10 @@
       <c r="B4" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="104" t="s">
+      <c r="C4" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="96"/>
+      <c r="D4" s="77"/>
       <c r="E4" s="36"/>
       <c r="F4" s="37"/>
     </row>
@@ -1839,8 +1815,8 @@
       <c r="B5" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="103"/>
-      <c r="D5" s="103"/>
+      <c r="C5" s="72"/>
+      <c r="D5" s="72"/>
       <c r="E5" s="36"/>
       <c r="F5" s="42"/>
     </row>
@@ -1849,18 +1825,18 @@
         <v>5</v>
       </c>
       <c r="B6" s="43" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" s="103"/>
-      <c r="D6" s="103"/>
+        <v>49</v>
+      </c>
+      <c r="C6" s="72"/>
+      <c r="D6" s="72"/>
       <c r="E6" s="36"/>
       <c r="F6" s="42"/>
     </row>
     <row r="7" spans="1:6" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="100">
+      <c r="A7" s="73">
         <v>6</v>
       </c>
-      <c r="B7" s="97" t="s">
+      <c r="B7" s="80" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="44" t="s">
@@ -1873,34 +1849,34 @@
       <c r="F7" s="37"/>
     </row>
     <row r="8" spans="1:6" s="30" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="101"/>
-      <c r="B8" s="98"/>
+      <c r="A8" s="74"/>
+      <c r="B8" s="81"/>
       <c r="C8" s="46"/>
       <c r="D8" s="47"/>
       <c r="E8" s="36"/>
       <c r="F8" s="37"/>
     </row>
     <row r="9" spans="1:6" s="30" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A9" s="101"/>
-      <c r="B9" s="98"/>
+      <c r="A9" s="74"/>
+      <c r="B9" s="81"/>
       <c r="C9" s="46"/>
       <c r="D9" s="47"/>
       <c r="E9" s="36"/>
       <c r="F9" s="37"/>
     </row>
     <row r="10" spans="1:6" s="30" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A10" s="102"/>
-      <c r="B10" s="99"/>
+      <c r="A10" s="75"/>
+      <c r="B10" s="82"/>
       <c r="C10" s="46"/>
       <c r="D10" s="47"/>
       <c r="E10" s="36"/>
       <c r="F10" s="37"/>
     </row>
     <row r="11" spans="1:6" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="100">
+      <c r="A11" s="73">
         <v>7</v>
       </c>
-      <c r="B11" s="97" t="s">
+      <c r="B11" s="80" t="s">
         <v>16</v>
       </c>
       <c r="C11" s="44" t="s">
@@ -1913,42 +1889,42 @@
       <c r="F11" s="37"/>
     </row>
     <row r="12" spans="1:6" s="30" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="101"/>
-      <c r="B12" s="98"/>
+      <c r="A12" s="74"/>
+      <c r="B12" s="81"/>
       <c r="C12" s="48"/>
       <c r="D12" s="47"/>
       <c r="E12" s="36"/>
       <c r="F12" s="37"/>
     </row>
     <row r="13" spans="1:6" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="101"/>
-      <c r="B13" s="98"/>
+      <c r="A13" s="74"/>
+      <c r="B13" s="81"/>
       <c r="C13" s="49"/>
       <c r="D13" s="49"/>
       <c r="E13" s="36"/>
       <c r="F13" s="37"/>
     </row>
     <row r="14" spans="1:6" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="101"/>
-      <c r="B14" s="98"/>
+      <c r="A14" s="74"/>
+      <c r="B14" s="81"/>
       <c r="C14" s="49"/>
       <c r="D14" s="49"/>
       <c r="E14" s="36"/>
       <c r="F14" s="37"/>
     </row>
     <row r="15" spans="1:6" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="102"/>
-      <c r="B15" s="99"/>
+      <c r="A15" s="75"/>
+      <c r="B15" s="82"/>
       <c r="C15" s="49"/>
       <c r="D15" s="49"/>
       <c r="E15" s="36"/>
       <c r="F15" s="37"/>
     </row>
     <row r="16" spans="1:6" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="100">
+      <c r="A16" s="73">
         <v>8</v>
       </c>
-      <c r="B16" s="97" t="s">
+      <c r="B16" s="80" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="44" t="s">
@@ -1961,42 +1937,42 @@
       <c r="F16" s="37"/>
     </row>
     <row r="17" spans="1:6" s="30" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A17" s="101"/>
-      <c r="B17" s="98"/>
+      <c r="A17" s="74"/>
+      <c r="B17" s="81"/>
       <c r="C17" s="48"/>
       <c r="D17" s="47"/>
       <c r="E17" s="36"/>
       <c r="F17" s="37"/>
     </row>
     <row r="18" spans="1:6" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="101"/>
-      <c r="B18" s="98"/>
+      <c r="A18" s="74"/>
+      <c r="B18" s="81"/>
       <c r="C18" s="49"/>
       <c r="D18" s="49"/>
       <c r="E18" s="36"/>
       <c r="F18" s="37"/>
     </row>
     <row r="19" spans="1:6" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="101"/>
-      <c r="B19" s="98"/>
+      <c r="A19" s="74"/>
+      <c r="B19" s="81"/>
       <c r="C19" s="49"/>
       <c r="D19" s="49"/>
       <c r="E19" s="36"/>
       <c r="F19" s="37"/>
     </row>
     <row r="20" spans="1:6" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="102"/>
-      <c r="B20" s="99"/>
+      <c r="A20" s="75"/>
+      <c r="B20" s="82"/>
       <c r="C20" s="49"/>
       <c r="D20" s="49"/>
       <c r="E20" s="36"/>
       <c r="F20" s="37"/>
     </row>
     <row r="21" spans="1:6" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="100">
+      <c r="A21" s="73">
         <v>8</v>
       </c>
-      <c r="B21" s="97" t="s">
+      <c r="B21" s="80" t="s">
         <v>17</v>
       </c>
       <c r="C21" s="44" t="s">
@@ -2009,42 +1985,42 @@
       <c r="F21" s="37"/>
     </row>
     <row r="22" spans="1:6" s="30" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A22" s="101"/>
-      <c r="B22" s="98"/>
+      <c r="A22" s="74"/>
+      <c r="B22" s="81"/>
       <c r="C22" s="48"/>
       <c r="D22" s="47"/>
       <c r="E22" s="36"/>
       <c r="F22" s="37"/>
     </row>
     <row r="23" spans="1:6" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="101"/>
-      <c r="B23" s="98"/>
+      <c r="A23" s="74"/>
+      <c r="B23" s="81"/>
       <c r="C23" s="49"/>
       <c r="D23" s="49"/>
       <c r="E23" s="36"/>
       <c r="F23" s="37"/>
     </row>
     <row r="24" spans="1:6" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="101"/>
-      <c r="B24" s="98"/>
+      <c r="A24" s="74"/>
+      <c r="B24" s="81"/>
       <c r="C24" s="49"/>
       <c r="D24" s="49"/>
       <c r="E24" s="36"/>
       <c r="F24" s="37"/>
     </row>
     <row r="25" spans="1:6" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="102"/>
-      <c r="B25" s="99"/>
+      <c r="A25" s="75"/>
+      <c r="B25" s="82"/>
       <c r="C25" s="49"/>
       <c r="D25" s="49"/>
       <c r="E25" s="36"/>
       <c r="F25" s="37"/>
     </row>
     <row r="26" spans="1:6" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="100">
+      <c r="A26" s="73">
         <v>8</v>
       </c>
-      <c r="B26" s="97" t="s">
+      <c r="B26" s="80" t="s">
         <v>19</v>
       </c>
       <c r="C26" s="44" t="s">
@@ -2057,32 +2033,32 @@
       <c r="F26" s="37"/>
     </row>
     <row r="27" spans="1:6" s="30" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A27" s="101"/>
-      <c r="B27" s="98"/>
+      <c r="A27" s="74"/>
+      <c r="B27" s="81"/>
       <c r="C27" s="48"/>
       <c r="D27" s="47"/>
       <c r="E27" s="36"/>
       <c r="F27" s="37"/>
     </row>
     <row r="28" spans="1:6" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="101"/>
-      <c r="B28" s="98"/>
+      <c r="A28" s="74"/>
+      <c r="B28" s="81"/>
       <c r="C28" s="49"/>
       <c r="D28" s="49"/>
       <c r="E28" s="36"/>
       <c r="F28" s="37"/>
     </row>
     <row r="29" spans="1:6" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="101"/>
-      <c r="B29" s="98"/>
+      <c r="A29" s="74"/>
+      <c r="B29" s="81"/>
       <c r="C29" s="49"/>
       <c r="D29" s="49"/>
       <c r="E29" s="36"/>
       <c r="F29" s="37"/>
     </row>
     <row r="30" spans="1:6" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="102"/>
-      <c r="B30" s="99"/>
+      <c r="A30" s="75"/>
+      <c r="B30" s="82"/>
       <c r="C30" s="49"/>
       <c r="D30" s="49"/>
       <c r="E30" s="36"/>
@@ -2095,8 +2071,8 @@
       <c r="B31" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="C31" s="104"/>
-      <c r="D31" s="96"/>
+      <c r="C31" s="76"/>
+      <c r="D31" s="77"/>
       <c r="E31" s="36"/>
       <c r="F31" s="37"/>
     </row>
@@ -2107,8 +2083,8 @@
       <c r="B32" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="C32" s="95"/>
-      <c r="D32" s="96"/>
+      <c r="C32" s="79"/>
+      <c r="D32" s="77"/>
       <c r="E32" s="36"/>
       <c r="F32" s="37"/>
     </row>
@@ -2210,14 +2186,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="A11:A15"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="B11:B15"/>
     <mergeCell ref="B7:B10"/>
@@ -2227,6 +2195,14 @@
     <mergeCell ref="B21:B25"/>
     <mergeCell ref="A26:A30"/>
     <mergeCell ref="B26:B30"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A11:A15"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2241,150 +2217,150 @@
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D5" sqref="D5"/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="2.25" style="60" customWidth="1"/>
-    <col min="2" max="2" width="4.25" style="61" customWidth="1"/>
-    <col min="3" max="3" width="18.125" style="61" customWidth="1"/>
-    <col min="4" max="4" width="17.25" style="60" customWidth="1"/>
-    <col min="5" max="5" width="13.625" style="61" customWidth="1"/>
-    <col min="6" max="6" width="31" style="61" customWidth="1"/>
-    <col min="7" max="7" width="73.125" style="60" customWidth="1"/>
-    <col min="8" max="8" width="42.625" style="60" customWidth="1"/>
-    <col min="9" max="16384" width="9.125" style="60"/>
+    <col min="1" max="1" width="2.25" style="59" customWidth="1"/>
+    <col min="2" max="2" width="4.25" style="60" customWidth="1"/>
+    <col min="3" max="3" width="18.125" style="60" customWidth="1"/>
+    <col min="4" max="4" width="17.25" style="59" customWidth="1"/>
+    <col min="5" max="5" width="13.625" style="60" customWidth="1"/>
+    <col min="6" max="6" width="31" style="60" customWidth="1"/>
+    <col min="7" max="7" width="73.125" style="59" customWidth="1"/>
+    <col min="8" max="8" width="42.625" style="59" customWidth="1"/>
+    <col min="9" max="16384" width="9.125" style="59"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="59"/>
+      <c r="C1" s="58"/>
     </row>
     <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="3" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="62" t="s">
+      <c r="B3" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="63" t="s">
+      <c r="C3" s="84" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="63" t="s">
+      <c r="D3" s="84" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="84" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="84" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="84" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="63" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" s="63" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3" s="63" t="s">
-        <v>42</v>
-      </c>
-      <c r="H3" s="64" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" ht="57" x14ac:dyDescent="0.4">
-      <c r="B4" s="65">
+      <c r="H3" s="85" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="48" x14ac:dyDescent="0.4">
+      <c r="B4" s="86">
         <f>ROW()-3</f>
         <v>1</v>
       </c>
-      <c r="C4" s="57" t="s">
+      <c r="C4" s="87" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="57" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" s="66" t="s">
+      <c r="D4" s="87" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="88" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="67"/>
-      <c r="G4" s="70" t="s">
-        <v>40</v>
-      </c>
-      <c r="H4" s="68"/>
+      <c r="F4" s="89"/>
+      <c r="G4" s="90" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4" s="91"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B5" s="65">
+      <c r="B5" s="86">
         <f t="shared" ref="B5:B9" si="0">ROW()-3</f>
         <v>2</v>
       </c>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57" t="s">
+      <c r="C5" s="87"/>
+      <c r="D5" s="87" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="66" t="s">
+      <c r="E5" s="88" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="67"/>
-      <c r="G5" s="57" t="s">
-        <v>41</v>
-      </c>
-      <c r="H5" s="68"/>
+      <c r="F5" s="89"/>
+      <c r="G5" s="87" t="s">
+        <v>53</v>
+      </c>
+      <c r="H5" s="91"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B6" s="65">
+      <c r="B6" s="86">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="C6" s="69"/>
-      <c r="D6" s="57"/>
-      <c r="E6" s="66"/>
-      <c r="F6" s="67"/>
-      <c r="G6" s="57"/>
-      <c r="H6" s="68"/>
+      <c r="C6" s="92"/>
+      <c r="D6" s="87"/>
+      <c r="E6" s="88"/>
+      <c r="F6" s="89"/>
+      <c r="G6" s="87"/>
+      <c r="H6" s="91"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B7" s="65">
+      <c r="B7" s="86">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C7" s="69"/>
-      <c r="D7" s="57"/>
-      <c r="E7" s="66"/>
-      <c r="F7" s="67"/>
-      <c r="G7" s="57"/>
-      <c r="H7" s="68"/>
+      <c r="C7" s="92"/>
+      <c r="D7" s="87"/>
+      <c r="E7" s="88"/>
+      <c r="F7" s="89"/>
+      <c r="G7" s="87"/>
+      <c r="H7" s="91"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B8" s="65">
+      <c r="B8" s="86">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C8" s="69"/>
-      <c r="D8" s="57"/>
-      <c r="E8" s="66"/>
-      <c r="F8" s="67"/>
-      <c r="G8" s="57"/>
-      <c r="H8" s="68"/>
+      <c r="C8" s="92"/>
+      <c r="D8" s="87"/>
+      <c r="E8" s="88"/>
+      <c r="F8" s="89"/>
+      <c r="G8" s="87"/>
+      <c r="H8" s="91"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B9" s="65">
+      <c r="B9" s="86">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C9" s="69"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="66"/>
-      <c r="F9" s="67"/>
-      <c r="G9" s="57"/>
-      <c r="H9" s="68"/>
+      <c r="C9" s="92"/>
+      <c r="D9" s="87"/>
+      <c r="E9" s="88"/>
+      <c r="F9" s="89"/>
+      <c r="G9" s="87"/>
+      <c r="H9" s="91"/>
     </row>
     <row r="10" spans="2:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B10" s="71" t="s">
+      <c r="B10" s="93" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="72" t="s">
+      <c r="C10" s="94" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="73"/>
-      <c r="E10" s="73"/>
-      <c r="F10" s="73"/>
-      <c r="G10" s="73"/>
-      <c r="H10" s="74"/>
+      <c r="D10" s="95"/>
+      <c r="E10" s="95"/>
+      <c r="F10" s="95"/>
+      <c r="G10" s="95"/>
+      <c r="H10" s="96"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3"/>
@@ -2416,90 +2392,88 @@
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="2.25" style="56" customWidth="1"/>
-    <col min="2" max="2" width="3.75" style="79" customWidth="1"/>
-    <col min="3" max="3" width="8.375" style="79" customWidth="1"/>
-    <col min="4" max="4" width="32.25" style="80" customWidth="1"/>
-    <col min="5" max="5" width="7.125" style="77" customWidth="1"/>
-    <col min="6" max="6" width="55.375" style="81" customWidth="1"/>
+    <col min="2" max="2" width="3.75" style="63" customWidth="1"/>
+    <col min="3" max="3" width="8.375" style="63" customWidth="1"/>
+    <col min="4" max="4" width="32.25" style="64" customWidth="1"/>
+    <col min="5" max="5" width="7.125" style="62" customWidth="1"/>
+    <col min="6" max="6" width="55.375" style="65" customWidth="1"/>
     <col min="7" max="7" width="38.875" style="56" customWidth="1"/>
     <col min="8" max="8" width="49" style="56" customWidth="1"/>
-    <col min="9" max="9" width="8.5" style="79" customWidth="1"/>
-    <col min="10" max="10" width="17.375" style="79" customWidth="1"/>
-    <col min="11" max="16384" width="9" style="56"/>
+    <col min="9" max="9" width="8.5" style="63" customWidth="1"/>
+    <col min="10" max="16384" width="9" style="56"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="60"/>
-      <c r="B1" s="82" t="s">
+      <c r="A1" s="59"/>
+      <c r="B1" s="66" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="56"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A2" s="59"/>
+      <c r="B2" s="69"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="61"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A3" s="59"/>
+      <c r="B3" s="97" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="98" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="98" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A2" s="60"/>
-      <c r="B2" s="85"/>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="87"/>
-      <c r="G2" s="87"/>
-      <c r="H2" s="87"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="56"/>
-    </row>
-    <row r="3" spans="1:10" ht="28.5" x14ac:dyDescent="0.4">
-      <c r="A3" s="60"/>
-      <c r="B3" s="88" t="s">
+      <c r="E3" s="98" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="98" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="89" t="s">
+      <c r="G3" s="97" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" s="97" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="89" t="s">
+      <c r="I3" s="97" t="s">
         <v>48</v>
       </c>
-      <c r="E3" s="89" t="s">
-        <v>46</v>
-      </c>
-      <c r="F3" s="89" t="s">
-        <v>49</v>
-      </c>
-      <c r="G3" s="88" t="s">
-        <v>50</v>
-      </c>
-      <c r="H3" s="88" t="s">
-        <v>51</v>
-      </c>
-      <c r="I3" s="76" t="s">
-        <v>52</v>
-      </c>
-      <c r="J3" s="77"/>
+      <c r="J3" s="99"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A4" s="60"/>
-      <c r="B4" s="90">
+      <c r="A4" s="59"/>
+      <c r="B4" s="100">
         <f>ROW()-3</f>
         <v>1</v>
       </c>
-      <c r="C4" s="66" t="s">
+      <c r="C4" s="88" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="91"/>
-      <c r="E4" s="92"/>
-      <c r="F4" s="93"/>
-      <c r="G4" s="57"/>
-      <c r="H4" s="94"/>
-      <c r="I4" s="78" t="str">
+      <c r="D4" s="101"/>
+      <c r="E4" s="102"/>
+      <c r="F4" s="103"/>
+      <c r="G4" s="87"/>
+      <c r="H4" s="104"/>
+      <c r="I4" s="105" t="str">
         <f ca="1">HYPERLINK("["&amp;SUBSTITUTE(CELL("filename"),TRIM(RIGHT(SUBSTITUTE(CELL("filename"),"\",REPT(" ",255)),255)),"")&amp;"Samples\No"&amp;B4&amp;".xlsx]","click")</f>
         <v>click</v>
       </c>
+      <c r="J4" s="99"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3"/>

</xml_diff>